<commit_message>
Rebuild and Fix CIPW！
</commit_message>
<xml_diff>
--- a/DataFileSamples/TAS REE Trace Pearce Harker CIPW/CIPW.xlsx
+++ b/DataFileSamples/TAS REE Trace Pearce Harker CIPW/CIPW.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/GeoCode/Python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/Documents/GitHub/GeoPyTool/DataFileSamples/TAS REE Trace Pearce Harker CIPW/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39280" yWindow="0" windowWidth="38400" windowHeight="21520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="工作表2" sheetId="3" r:id="rId4"/>
     <sheet name="工作表3" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525" iterateCount="200" iterateDelta="9.9999999999999995E-7" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateCount="200" iterateDelta="9.9999999999999995E-7" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="370">
   <si>
     <t>Name</t>
   </si>
@@ -1187,6 +1187,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1200,6 +1201,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1213,6 +1215,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1226,6 +1229,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1239,6 +1243,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1252,6 +1257,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1265,6 +1271,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1278,6 +1285,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1291,6 +1299,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1304,6 +1313,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1317,6 +1327,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1330,6 +1341,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1343,6 +1355,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1356,6 +1369,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1369,6 +1383,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1382,6 +1397,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1395,6 +1411,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1408,6 +1425,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1421,6 +1439,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1434,6 +1453,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1447,6 +1467,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1460,6 +1481,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1473,6 +1495,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1486,6 +1509,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1499,6 +1523,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1512,6 +1537,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1525,6 +1551,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1538,6 +1565,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1551,6 +1579,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1564,6 +1593,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1577,6 +1607,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1590,6 +1621,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1603,6 +1635,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1616,6 +1649,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1629,6 +1663,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1642,6 +1677,7 @@
         <sz val="12"/>
         <color rgb="FFCE9178"/>
         <rFont val="Menlo"/>
+        <family val="2"/>
       </rPr>
       <t>'.</t>
     </r>
@@ -1867,17 +1903,36 @@
     <t>Zr</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <t xml:space="preserve"> BARK4</t>
+  </si>
+  <si>
+    <t>BARKER-TAB-4-4-&amp;-4-7</t>
+  </si>
+  <si>
+    <t>red</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="4">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="178" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1904,6 +1959,7 @@
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1916,6 +1972,7 @@
       <sz val="14"/>
       <color rgb="FF4F81BD"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
@@ -1936,16 +1993,19 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Abadi MT Condensed Extra Bold"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFD4D4D4"/>
       <name val="Menlo"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFCE9178"/>
       <name val="Menlo"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2004,8 +2064,15 @@
       <color theme="0"/>
       <name val="Times Roman"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2040,6 +2107,17 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightGray">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
   </fills>
@@ -2161,7 +2239,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2249,6 +2327,24 @@
     <xf numFmtId="178" fontId="18" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="18" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="178" fontId="18" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2263,6 +2359,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2526,18 +2625,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD293"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
     <col min="28" max="28" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="28" customFormat="1" ht="18">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -2632,7 +2731,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31">
       <c r="A2" s="37" t="s">
         <v>349</v>
       </c>
@@ -2724,6 +2823,101 @@
         <v>0</v>
       </c>
       <c r="AE2" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>367</v>
+      </c>
+      <c r="G3" s="39">
+        <v>20</v>
+      </c>
+      <c r="H3" s="39">
+        <v>0.6</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>369</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>368</v>
+      </c>
+      <c r="K3" s="43">
+        <v>44.309090909090898</v>
+      </c>
+      <c r="L3" s="43">
+        <v>2.7</v>
+      </c>
+      <c r="M3" s="43">
+        <v>13.263636363636399</v>
+      </c>
+      <c r="N3" s="43">
+        <v>13.2909090909091</v>
+      </c>
+      <c r="O3" s="43">
+        <v>0</v>
+      </c>
+      <c r="P3" s="44">
+        <v>0.13</v>
+      </c>
+      <c r="Q3" s="43">
+        <v>9.9963636363636397</v>
+      </c>
+      <c r="R3" s="44">
+        <v>5.8154545454545401</v>
+      </c>
+      <c r="S3" s="43">
+        <v>2.8036363636363602</v>
+      </c>
+      <c r="T3" s="43">
+        <v>1.4463636363636401</v>
+      </c>
+      <c r="U3" s="44">
+        <v>0.47</v>
+      </c>
+      <c r="V3" s="45">
+        <v>0</v>
+      </c>
+      <c r="W3" s="46">
+        <v>0</v>
+      </c>
+      <c r="X3" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="45">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="47">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="47">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="47">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="47">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2741,9 +2935,9 @@
       <selection sqref="A1:Y120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2820,7 +3014,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="18">
       <c r="A2" s="13" t="s">
         <v>179</v>
       </c>
@@ -2897,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="18">
       <c r="A3" s="13" t="s">
         <v>182</v>
       </c>
@@ -2974,7 +3168,7 @@
         <v>3.9999999100000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="18">
       <c r="A4" s="13" t="s">
         <v>183</v>
       </c>
@@ -3051,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="18">
       <c r="A5" s="13" t="s">
         <v>185</v>
       </c>
@@ -3128,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="18">
       <c r="A6" s="13" t="s">
         <v>187</v>
       </c>
@@ -3205,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="18">
       <c r="A7" s="13" t="s">
         <v>188</v>
       </c>
@@ -3282,7 +3476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="18">
       <c r="A8" s="13" t="s">
         <v>189</v>
       </c>
@@ -3359,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="18">
       <c r="A9" s="13" t="s">
         <v>190</v>
       </c>
@@ -3436,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="18">
       <c r="A10" s="13" t="s">
         <v>191</v>
       </c>
@@ -3513,7 +3707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="18">
       <c r="A11" s="13" t="s">
         <v>192</v>
       </c>
@@ -3590,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="18">
       <c r="A12" s="13" t="s">
         <v>193</v>
       </c>
@@ -3667,7 +3861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" ht="18">
       <c r="A13" s="13" t="s">
         <v>194</v>
       </c>
@@ -3744,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="18">
       <c r="A14" s="13" t="s">
         <v>195</v>
       </c>
@@ -3821,7 +4015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="18">
       <c r="A15" s="13" t="s">
         <v>196</v>
       </c>
@@ -3898,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="18">
       <c r="A16" s="13" t="s">
         <v>197</v>
       </c>
@@ -3975,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="18">
       <c r="A17" s="13" t="s">
         <v>198</v>
       </c>
@@ -4052,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="18">
       <c r="A18" s="13" t="s">
         <v>200</v>
       </c>
@@ -4129,7 +4323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="18">
       <c r="A19" s="13" t="s">
         <v>201</v>
       </c>
@@ -4206,7 +4400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="18">
       <c r="A20" s="13" t="s">
         <v>202</v>
       </c>
@@ -4283,7 +4477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="18">
       <c r="A21" s="13" t="s">
         <v>203</v>
       </c>
@@ -4360,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="18">
       <c r="A22" s="13" t="s">
         <v>204</v>
       </c>
@@ -4437,7 +4631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="18">
       <c r="A23" s="13" t="s">
         <v>205</v>
       </c>
@@ -4514,7 +4708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="18">
       <c r="A24" s="13" t="s">
         <v>207</v>
       </c>
@@ -4591,7 +4785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="18">
       <c r="A25" s="13" t="s">
         <v>208</v>
       </c>
@@ -4668,7 +4862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="18">
       <c r="A26" s="13" t="s">
         <v>209</v>
       </c>
@@ -4745,7 +4939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="18">
       <c r="A27" s="13" t="s">
         <v>210</v>
       </c>
@@ -4822,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="18">
       <c r="A28" s="13" t="s">
         <v>211</v>
       </c>
@@ -4899,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="18">
       <c r="A29" s="13" t="s">
         <v>212</v>
       </c>
@@ -4976,7 +5170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="18">
       <c r="A30" s="13" t="s">
         <v>213</v>
       </c>
@@ -5053,7 +5247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="18">
       <c r="A31" s="13" t="s">
         <v>214</v>
       </c>
@@ -5130,7 +5324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="18">
       <c r="A32" s="13" t="s">
         <v>215</v>
       </c>
@@ -5207,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="18">
       <c r="A33" s="13" t="s">
         <v>216</v>
       </c>
@@ -5284,7 +5478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="18">
       <c r="A34" s="13" t="s">
         <v>217</v>
       </c>
@@ -5361,7 +5555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="18">
       <c r="A35" s="13" t="s">
         <v>218</v>
       </c>
@@ -5438,7 +5632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="18">
       <c r="A36" s="13" t="s">
         <v>219</v>
       </c>
@@ -5515,7 +5709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" ht="18">
       <c r="A37" s="13" t="s">
         <v>220</v>
       </c>
@@ -5592,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" ht="18">
       <c r="A38" s="13" t="s">
         <v>221</v>
       </c>
@@ -5669,7 +5863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="18">
       <c r="A39" s="13" t="s">
         <v>222</v>
       </c>
@@ -5746,7 +5940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="18">
       <c r="A40" s="13" t="s">
         <v>223</v>
       </c>
@@ -5823,7 +6017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" ht="18">
       <c r="A41" s="13" t="s">
         <v>224</v>
       </c>
@@ -5900,7 +6094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" ht="18">
       <c r="A42" s="13" t="s">
         <v>225</v>
       </c>
@@ -5977,7 +6171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" ht="18">
       <c r="A43" s="13" t="s">
         <v>226</v>
       </c>
@@ -6054,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" ht="18">
       <c r="A44" s="13" t="s">
         <v>227</v>
       </c>
@@ -6131,7 +6325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" ht="18">
       <c r="A45" s="13" t="s">
         <v>228</v>
       </c>
@@ -6208,7 +6402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" ht="18">
       <c r="A46" s="13" t="s">
         <v>229</v>
       </c>
@@ -6285,7 +6479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="18">
       <c r="A47" s="13" t="s">
         <v>230</v>
       </c>
@@ -6362,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" ht="18">
       <c r="A48" s="13" t="s">
         <v>231</v>
       </c>
@@ -6439,7 +6633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="18">
       <c r="A49" s="13" t="s">
         <v>232</v>
       </c>
@@ -6516,7 +6710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="18">
       <c r="A50" s="13" t="s">
         <v>233</v>
       </c>
@@ -6593,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="18">
       <c r="A51" s="13" t="s">
         <v>234</v>
       </c>
@@ -6670,7 +6864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="18">
       <c r="A52" s="13" t="s">
         <v>235</v>
       </c>
@@ -6747,7 +6941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" ht="18">
       <c r="A53" s="13" t="s">
         <v>236</v>
       </c>
@@ -6824,7 +7018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" ht="18">
       <c r="A54" s="13" t="s">
         <v>237</v>
       </c>
@@ -6901,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" ht="18">
       <c r="A55" s="13" t="s">
         <v>238</v>
       </c>
@@ -6978,7 +7172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" ht="18">
       <c r="A56" s="13" t="s">
         <v>240</v>
       </c>
@@ -7055,7 +7249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" ht="18">
       <c r="A57" s="13" t="s">
         <v>241</v>
       </c>
@@ -7132,7 +7326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" ht="18">
       <c r="A58" s="13" t="s">
         <v>242</v>
       </c>
@@ -7209,7 +7403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" ht="18">
       <c r="A59" s="13" t="s">
         <v>243</v>
       </c>
@@ -7286,7 +7480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" ht="18">
       <c r="A60" s="13" t="s">
         <v>244</v>
       </c>
@@ -7363,7 +7557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" ht="18">
       <c r="A61" s="13" t="s">
         <v>245</v>
       </c>
@@ -7440,7 +7634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" ht="18">
       <c r="A62" s="13" t="s">
         <v>246</v>
       </c>
@@ -7517,7 +7711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" ht="18">
       <c r="A63" s="13" t="s">
         <v>247</v>
       </c>
@@ -7594,7 +7788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" ht="18">
       <c r="A64" s="13" t="s">
         <v>248</v>
       </c>
@@ -7671,7 +7865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" ht="18">
       <c r="A65" s="13" t="s">
         <v>249</v>
       </c>
@@ -7748,7 +7942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" ht="18">
       <c r="A66" s="13" t="s">
         <v>250</v>
       </c>
@@ -7825,7 +8019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" ht="18">
       <c r="A67" s="13" t="s">
         <v>251</v>
       </c>
@@ -7902,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" ht="18">
       <c r="A68" s="13" t="s">
         <v>253</v>
       </c>
@@ -7979,7 +8173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" ht="18">
       <c r="A69" s="13" t="s">
         <v>254</v>
       </c>
@@ -8056,7 +8250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" ht="18">
       <c r="A70" s="13" t="s">
         <v>255</v>
       </c>
@@ -8133,7 +8327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" ht="18">
       <c r="A71" s="13" t="s">
         <v>256</v>
       </c>
@@ -8210,7 +8404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" ht="18">
       <c r="A72" s="13" t="s">
         <v>257</v>
       </c>
@@ -8287,7 +8481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" ht="18">
       <c r="A73" s="13" t="s">
         <v>258</v>
       </c>
@@ -8364,7 +8558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" ht="18">
       <c r="A74" s="13" t="s">
         <v>259</v>
       </c>
@@ -8441,7 +8635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:25" ht="18">
       <c r="A75" s="13" t="s">
         <v>260</v>
       </c>
@@ -8518,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25" ht="18">
       <c r="A76" s="13" t="s">
         <v>261</v>
       </c>
@@ -8595,7 +8789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:25" ht="18">
       <c r="A77" s="13" t="s">
         <v>262</v>
       </c>
@@ -8672,7 +8866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:25" ht="18">
       <c r="A78" s="13" t="s">
         <v>263</v>
       </c>
@@ -8749,7 +8943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:25" ht="18">
       <c r="A79" s="13" t="s">
         <v>265</v>
       </c>
@@ -8826,7 +9020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:25" ht="18">
       <c r="A80" s="13" t="s">
         <v>266</v>
       </c>
@@ -8903,7 +9097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:25" ht="18">
       <c r="A81" s="13" t="s">
         <v>267</v>
       </c>
@@ -8980,7 +9174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:25" ht="18">
       <c r="A82" s="13" t="s">
         <v>268</v>
       </c>
@@ -9057,7 +9251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:25" ht="18">
       <c r="A83" s="13" t="s">
         <v>269</v>
       </c>
@@ -9134,7 +9328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:25" ht="18">
       <c r="A84" s="13" t="s">
         <v>270</v>
       </c>
@@ -9211,7 +9405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:25" ht="18">
       <c r="A85" s="13" t="s">
         <v>271</v>
       </c>
@@ -9288,7 +9482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:25" ht="18">
       <c r="A86" s="13" t="s">
         <v>272</v>
       </c>
@@ -9365,7 +9559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:25" ht="18">
       <c r="A87" s="13" t="s">
         <v>273</v>
       </c>
@@ -9442,7 +9636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:25" ht="18">
       <c r="A88" s="13" t="s">
         <v>274</v>
       </c>
@@ -9519,7 +9713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:25" ht="18">
       <c r="A89" s="13" t="s">
         <v>275</v>
       </c>
@@ -9596,7 +9790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:25" ht="18">
       <c r="A90" s="13" t="s">
         <v>276</v>
       </c>
@@ -9673,7 +9867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:25" ht="18">
       <c r="A91" s="13" t="s">
         <v>278</v>
       </c>
@@ -9750,7 +9944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:25" ht="18">
       <c r="A92" s="13" t="s">
         <v>279</v>
       </c>
@@ -9827,7 +10021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:25" ht="18">
       <c r="A93" s="13" t="s">
         <v>280</v>
       </c>
@@ -9904,7 +10098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:25" ht="18">
       <c r="A94" s="13" t="s">
         <v>281</v>
       </c>
@@ -9981,7 +10175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:25" ht="18">
       <c r="A95" s="13" t="s">
         <v>282</v>
       </c>
@@ -10058,7 +10252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:25" ht="18">
       <c r="A96" s="13" t="s">
         <v>283</v>
       </c>
@@ -10135,7 +10329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:25" ht="18">
       <c r="A97" s="13" t="s">
         <v>284</v>
       </c>
@@ -10212,7 +10406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:25" ht="18">
       <c r="A98" s="13" t="s">
         <v>285</v>
       </c>
@@ -10289,7 +10483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:25" ht="18">
       <c r="A99" s="13" t="s">
         <v>286</v>
       </c>
@@ -10366,7 +10560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:25" ht="18">
       <c r="A100" s="13" t="s">
         <v>287</v>
       </c>
@@ -10443,7 +10637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:25" ht="18">
       <c r="A101" s="13" t="s">
         <v>288</v>
       </c>
@@ -10520,7 +10714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:25" ht="18">
       <c r="A102" s="13" t="s">
         <v>290</v>
       </c>
@@ -10597,7 +10791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:25" ht="18">
       <c r="A103" s="13" t="s">
         <v>292</v>
       </c>
@@ -10674,7 +10868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:25" ht="18">
       <c r="A104" s="13" t="s">
         <v>293</v>
       </c>
@@ -10751,7 +10945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:25" ht="18">
       <c r="A105" s="13" t="s">
         <v>294</v>
       </c>
@@ -10828,7 +11022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:25" ht="18">
       <c r="A106" s="13" t="s">
         <v>296</v>
       </c>
@@ -10905,7 +11099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:25" ht="18">
       <c r="A107" s="13" t="s">
         <v>297</v>
       </c>
@@ -10982,7 +11176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:25" ht="18">
       <c r="A108" s="13" t="s">
         <v>298</v>
       </c>
@@ -11059,7 +11253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:25" ht="18">
       <c r="A109" s="13" t="s">
         <v>228</v>
       </c>
@@ -11136,7 +11330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:25" ht="18">
       <c r="A110" s="13" t="s">
         <v>201</v>
       </c>
@@ -11213,7 +11407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:25" ht="18">
       <c r="A111" s="13" t="s">
         <v>201</v>
       </c>
@@ -11290,7 +11484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:25" ht="18">
       <c r="A112" s="13" t="s">
         <v>300</v>
       </c>
@@ -11367,7 +11561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:25" ht="18">
       <c r="A113" s="13" t="s">
         <v>203</v>
       </c>
@@ -11444,7 +11638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:25" ht="18">
       <c r="A114" s="13" t="s">
         <v>228</v>
       </c>
@@ -11521,7 +11715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:25" ht="18">
       <c r="A115" s="13" t="s">
         <v>224</v>
       </c>
@@ -11598,7 +11792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:25" ht="18">
       <c r="A116" s="13" t="s">
         <v>221</v>
       </c>
@@ -11675,7 +11869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:25" ht="18">
       <c r="A117" s="13" t="s">
         <v>203</v>
       </c>
@@ -11752,7 +11946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:25" ht="18">
       <c r="A118" s="13" t="s">
         <v>211</v>
       </c>
@@ -11829,7 +12023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:25" ht="18">
       <c r="A119" s="13" t="s">
         <v>302</v>
       </c>
@@ -11906,7 +12100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:25" ht="18">
       <c r="A120" s="13" t="s">
         <v>304</v>
       </c>
@@ -11997,9 +12191,9 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:63" ht="18">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -12190,7 +12384,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:63" ht="18">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
@@ -12377,7 +12571,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:63" ht="18">
       <c r="A3" s="2" t="s">
         <v>93</v>
       </c>
@@ -12568,7 +12762,7 @@
         <v>2.15784062884704</v>
       </c>
     </row>
-    <row r="4" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:63" ht="18">
       <c r="A4" s="2" t="s">
         <v>95</v>
       </c>
@@ -12759,7 +12953,7 @@
         <v>8.7385798932775902</v>
       </c>
     </row>
-    <row r="5" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:63" ht="18">
       <c r="A5" s="2" t="s">
         <v>97</v>
       </c>
@@ -12950,7 +13144,7 @@
         <v>10.0310838280254</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:63" ht="18">
       <c r="A6" s="2" t="s">
         <v>99</v>
       </c>
@@ -13141,7 +13335,7 @@
         <v>13.026946990491</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:63" ht="18">
       <c r="A7" s="2" t="s">
         <v>101</v>
       </c>
@@ -13332,7 +13526,7 @@
         <v>5.56113101049388</v>
       </c>
     </row>
-    <row r="8" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:63" ht="18">
       <c r="A8" s="2" t="s">
         <v>103</v>
       </c>
@@ -13523,7 +13717,7 @@
         <v>0.66265318547338503</v>
       </c>
     </row>
-    <row r="9" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:63" ht="18">
       <c r="A9" s="2" t="s">
         <v>105</v>
       </c>
@@ -13714,7 +13908,7 @@
         <v>1.1111123753084</v>
       </c>
     </row>
-    <row r="10" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:63" ht="18">
       <c r="A10" s="2" t="s">
         <v>107</v>
       </c>
@@ -13905,7 +14099,7 @@
         <v>0.88088163223808902</v>
       </c>
     </row>
-    <row r="11" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:63" ht="18">
       <c r="A11" s="2" t="s">
         <v>109</v>
       </c>
@@ -14096,7 +14290,7 @@
         <v>5.47</v>
       </c>
     </row>
-    <row r="12" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:63" ht="18">
       <c r="A12" s="2" t="s">
         <v>111</v>
       </c>
@@ -14287,7 +14481,7 @@
         <v>4.4264381713390897</v>
       </c>
     </row>
-    <row r="13" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:63" ht="18">
       <c r="A13" s="2" t="s">
         <v>113</v>
       </c>
@@ -14478,7 +14672,7 @@
         <v>5.47777024111699</v>
       </c>
     </row>
-    <row r="14" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:63" ht="18">
       <c r="A14" s="2" t="s">
         <v>115</v>
       </c>
@@ -14669,7 +14863,7 @@
         <v>12.848877407687599</v>
       </c>
     </row>
-    <row r="15" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:63" ht="18">
       <c r="A15" s="2" t="s">
         <v>96</v>
       </c>
@@ -14860,7 +15054,7 @@
         <v>8.7207607323767906</v>
       </c>
     </row>
-    <row r="16" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:63" ht="18">
       <c r="A16" s="2" t="s">
         <v>118</v>
       </c>
@@ -15051,7 +15245,7 @@
         <v>4.9849500531286903</v>
       </c>
     </row>
-    <row r="17" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:63" ht="18">
       <c r="A17" s="2" t="s">
         <v>120</v>
       </c>
@@ -15242,7 +15436,7 @@
         <v>9.72035834098625</v>
       </c>
     </row>
-    <row r="18" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:63" ht="18">
       <c r="A18" s="2" t="s">
         <v>122</v>
       </c>
@@ -15433,7 +15627,7 @@
         <v>3.9152873084225401</v>
       </c>
     </row>
-    <row r="19" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:63" ht="18">
       <c r="A19" s="2" t="s">
         <v>124</v>
       </c>
@@ -15624,7 +15818,7 @@
         <v>6.0414798391609503</v>
       </c>
     </row>
-    <row r="20" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:63" ht="18">
       <c r="A20" s="2" t="s">
         <v>126</v>
       </c>
@@ -15815,7 +16009,7 @@
         <v>0.659340327683554</v>
       </c>
     </row>
-    <row r="21" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:63" ht="18">
       <c r="A21" s="2" t="s">
         <v>128</v>
       </c>
@@ -16006,7 +16200,7 @@
         <v>7.1371939019769099</v>
       </c>
     </row>
-    <row r="22" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:63" ht="18">
       <c r="A22" s="2" t="s">
         <v>130</v>
       </c>
@@ -16197,7 +16391,7 @@
         <v>2.5586627580250298</v>
       </c>
     </row>
-    <row r="23" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:63" ht="18">
       <c r="A23" s="2" t="s">
         <v>132</v>
       </c>
@@ -16388,7 +16582,7 @@
         <v>0.57768645799771001</v>
       </c>
     </row>
-    <row r="24" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:63" ht="18">
       <c r="A24" s="2" t="s">
         <v>98</v>
       </c>
@@ -16579,7 +16773,7 @@
         <v>10.0102981208738</v>
       </c>
     </row>
-    <row r="25" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:63" ht="18">
       <c r="A25" s="2" t="s">
         <v>135</v>
       </c>
@@ -16770,7 +16964,7 @@
         <v>14.8517503588353</v>
       </c>
     </row>
-    <row r="26" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:63" ht="18">
       <c r="A26" s="2" t="s">
         <v>137</v>
       </c>
@@ -16961,7 +17155,7 @@
         <v>5.2112239545011603</v>
       </c>
     </row>
-    <row r="27" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:63" ht="18">
       <c r="A27" s="2" t="s">
         <v>139</v>
       </c>
@@ -17152,7 +17346,7 @@
         <v>36.479999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:63" ht="18">
       <c r="A28" s="2" t="s">
         <v>141</v>
       </c>
@@ -17343,7 +17537,7 @@
         <v>5.1939848589910298</v>
       </c>
     </row>
-    <row r="29" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:63" ht="18">
       <c r="A29" s="2" t="s">
         <v>143</v>
       </c>
@@ -17534,7 +17728,7 @@
         <v>3.16952258051642</v>
       </c>
     </row>
-    <row r="30" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:63" ht="18">
       <c r="A30" s="2" t="s">
         <v>145</v>
       </c>
@@ -17725,7 +17919,7 @@
         <v>25.28</v>
       </c>
     </row>
-    <row r="31" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:63" ht="18">
       <c r="A31" s="2" t="s">
         <v>147</v>
       </c>
@@ -17916,7 +18110,7 @@
         <v>2.97190090767949</v>
       </c>
     </row>
-    <row r="32" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:63" ht="18">
       <c r="A32" s="2" t="s">
         <v>149</v>
       </c>
@@ -18107,7 +18301,7 @@
         <v>1.31867943477211</v>
       </c>
     </row>
-    <row r="33" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:63" ht="18">
       <c r="A33" s="2" t="s">
         <v>100</v>
       </c>
@@ -18298,7 +18492,7 @@
         <v>13.0790223670034</v>
       </c>
     </row>
-    <row r="34" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:63" ht="18">
       <c r="A34" s="2" t="s">
         <v>152</v>
       </c>
@@ -18489,7 +18683,7 @@
         <v>1.3581550598310701</v>
       </c>
     </row>
-    <row r="35" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:63" ht="18">
       <c r="A35" s="2" t="s">
         <v>154</v>
       </c>
@@ -18680,7 +18874,7 @@
         <v>1.2990986220327401</v>
       </c>
     </row>
-    <row r="36" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:63" ht="18">
       <c r="A36" s="2" t="s">
         <v>156</v>
       </c>
@@ -18871,7 +19065,7 @@
         <v>1.2525411152382</v>
       </c>
     </row>
-    <row r="37" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:63" ht="18">
       <c r="A37" s="2" t="s">
         <v>158</v>
       </c>
@@ -19062,7 +19256,7 @@
         <v>3.6906420371480699</v>
       </c>
     </row>
-    <row r="38" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:63" ht="18">
       <c r="A38" s="2" t="s">
         <v>160</v>
       </c>
@@ -19253,7 +19447,7 @@
         <v>12.9682868048604</v>
       </c>
     </row>
-    <row r="39" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:63" ht="18">
       <c r="A39" s="2" t="s">
         <v>162</v>
       </c>
@@ -19444,7 +19638,7 @@
         <v>1.21119375872206</v>
       </c>
     </row>
-    <row r="40" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:63" ht="18">
       <c r="A40" s="2" t="s">
         <v>164</v>
       </c>
@@ -19635,7 +19829,7 @@
         <v>3.9514015275578598</v>
       </c>
     </row>
-    <row r="41" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:63" ht="18">
       <c r="A41" s="2" t="s">
         <v>166</v>
       </c>
@@ -19826,7 +20020,7 @@
         <v>15.0002229317294</v>
       </c>
     </row>
-    <row r="42" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:63" ht="18">
       <c r="A42" s="2" t="s">
         <v>102</v>
       </c>
@@ -20017,7 +20211,7 @@
         <v>5.5755830656444498</v>
       </c>
     </row>
-    <row r="43" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:63" ht="18">
       <c r="A43" s="2" t="s">
         <v>169</v>
       </c>
@@ -20208,7 +20402,7 @@
         <v>1.2374287880146999</v>
       </c>
     </row>
-    <row r="44" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:63" ht="18">
       <c r="A44" s="2" t="s">
         <v>171</v>
       </c>
@@ -20399,7 +20593,7 @@
         <v>2.5874107862032898</v>
       </c>
     </row>
-    <row r="45" spans="1:63" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:63" ht="18">
       <c r="A45" s="2" t="s">
         <v>173</v>
       </c>
@@ -20604,14 +20798,14 @@
       <selection activeCell="C38" sqref="A2:C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="B1" s="15" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>343</v>
       </c>
@@ -20619,7 +20813,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="16" t="s">
         <v>343</v>
       </c>
@@ -20627,7 +20821,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="16" t="s">
         <v>343</v>
       </c>
@@ -20635,7 +20829,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="16" t="s">
         <v>343</v>
       </c>
@@ -20643,7 +20837,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="16" t="s">
         <v>343</v>
       </c>
@@ -20651,7 +20845,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="16" t="s">
         <v>343</v>
       </c>
@@ -20659,7 +20853,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="16" t="s">
         <v>343</v>
       </c>
@@ -20667,7 +20861,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="16" t="s">
         <v>343</v>
       </c>
@@ -20675,7 +20869,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="16" t="s">
         <v>343</v>
       </c>
@@ -20683,7 +20877,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="16" t="s">
         <v>343</v>
       </c>
@@ -20691,7 +20885,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="16" t="s">
         <v>343</v>
       </c>
@@ -20699,7 +20893,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="16" t="s">
         <v>343</v>
       </c>
@@ -20707,7 +20901,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="16" t="s">
         <v>343</v>
       </c>
@@ -20715,7 +20909,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="16" t="s">
         <v>343</v>
       </c>
@@ -20723,7 +20917,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="16" t="s">
         <v>343</v>
       </c>
@@ -20731,7 +20925,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="16" t="s">
         <v>343</v>
       </c>
@@ -20739,7 +20933,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="16" t="s">
         <v>343</v>
       </c>
@@ -20747,7 +20941,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="16" t="s">
         <v>343</v>
       </c>
@@ -20755,7 +20949,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="16" t="s">
         <v>343</v>
       </c>
@@ -20763,7 +20957,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="16" t="s">
         <v>343</v>
       </c>
@@ -20771,7 +20965,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="16" t="s">
         <v>343</v>
       </c>
@@ -20779,7 +20973,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="16" t="s">
         <v>343</v>
       </c>
@@ -20787,7 +20981,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="16" t="s">
         <v>343</v>
       </c>
@@ -20795,7 +20989,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="16" t="s">
         <v>343</v>
       </c>
@@ -20803,7 +20997,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="16" t="s">
         <v>343</v>
       </c>
@@ -20811,7 +21005,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="16" t="s">
         <v>343</v>
       </c>
@@ -20819,7 +21013,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="16" t="s">
         <v>343</v>
       </c>
@@ -20827,7 +21021,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="16" t="s">
         <v>343</v>
       </c>
@@ -20835,7 +21029,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" s="16" t="s">
         <v>343</v>
       </c>
@@ -20843,7 +21037,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="16" t="s">
         <v>343</v>
       </c>
@@ -20851,7 +21045,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" s="16" t="s">
         <v>343</v>
       </c>
@@ -20859,7 +21053,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="A33" s="16" t="s">
         <v>343</v>
       </c>
@@ -20867,7 +21061,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="A34" s="16" t="s">
         <v>343</v>
       </c>
@@ -20875,7 +21069,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="A35" s="16" t="s">
         <v>343</v>
       </c>
@@ -20883,7 +21077,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2">
       <c r="A36" s="16" t="s">
         <v>343</v>
       </c>
@@ -20891,7 +21085,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="16" t="s">
         <v>343</v>
       </c>
@@ -20899,7 +21093,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="A38" s="16" t="s">
         <v>343</v>
       </c>
@@ -20907,67 +21101,67 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="A39" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="A40" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2">
       <c r="A41" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2">
       <c r="A42" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="A43" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="A44" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2">
       <c r="A45" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2">
       <c r="A46" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2">
       <c r="A47" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2">
       <c r="A48" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="16" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="16" t="s">
         <v>343</v>
       </c>
@@ -20989,9 +21183,9 @@
       <selection sqref="A1:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="17" t="s">
         <v>82</v>
       </c>
@@ -21002,7 +21196,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="20" t="s">
         <v>88</v>
       </c>
@@ -21013,7 +21207,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="20" t="s">
         <v>83</v>
       </c>
@@ -21024,7 +21218,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="20" t="s">
         <v>84</v>
       </c>
@@ -21035,7 +21229,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
@@ -21046,7 +21240,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="20" t="s">
         <v>14</v>
       </c>
@@ -21057,7 +21251,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="20" t="s">
         <v>15</v>
       </c>
@@ -21068,7 +21262,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="20" t="s">
         <v>16</v>
       </c>
@@ -21079,7 +21273,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="20" t="s">
         <v>85</v>
       </c>
@@ -21090,7 +21284,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="20" t="s">
         <v>86</v>
       </c>
@@ -21101,7 +21295,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="20" t="s">
         <v>87</v>
       </c>
@@ -21112,7 +21306,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="20" t="s">
         <v>344</v>
       </c>
@@ -21123,7 +21317,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="20" t="s">
         <v>345</v>
       </c>
@@ -21132,7 +21326,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="20" t="s">
         <v>53</v>
       </c>
@@ -21143,7 +21337,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="20" t="s">
         <v>346</v>
       </c>
@@ -21154,7 +21348,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="20" t="s">
         <v>347</v>
       </c>
@@ -21165,7 +21359,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="20" t="s">
         <v>58</v>
       </c>
@@ -21176,7 +21370,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="20" t="s">
         <v>37</v>
       </c>
@@ -21187,7 +21381,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="20" t="s">
         <v>50</v>
       </c>
@@ -21198,7 +21392,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="20" t="s">
         <v>41</v>
       </c>
@@ -21209,7 +21403,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="25" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
update CIA and ICV
</commit_message>
<xml_diff>
--- a/DataFileSamples/TAS REE Trace Pearce Harker CIPW/CIPW.xlsx
+++ b/DataFileSamples/TAS REE Trace Pearce Harker CIPW/CIPW.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/Documents/GitHub/GeoPyTool/DataFileSamples/TAS REE Trace Pearce Harker CIPW/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{011B2223-B612-734F-9FB0-E93394DDE9CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="373">
   <si>
     <t>Name</t>
   </si>
@@ -1720,20 +1721,6 @@
   </si>
   <si>
     <r>
-      <t>SiO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Times Roman"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>TiO</t>
     </r>
     <r>
@@ -1921,11 +1908,46 @@
     <t>-</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>SiO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Times Roman"/>
+      </rPr>
+      <t xml:space="preserve">  wt%</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>S (ppm)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>F（ppm）</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CaO （质量分数）</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
@@ -2348,7 +2370,7 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="常规 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
@@ -2624,11 +2646,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -2668,16 +2690,16 @@
         <v>8</v>
       </c>
       <c r="K1" s="33" t="s">
+        <v>369</v>
+      </c>
+      <c r="L1" s="33" t="s">
         <v>353</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>354</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>355</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>356</v>
       </c>
       <c r="O1" s="33" t="s">
         <v>13</v>
@@ -2689,16 +2711,16 @@
         <v>15</v>
       </c>
       <c r="R1" s="33" t="s">
-        <v>16</v>
+        <v>372</v>
       </c>
       <c r="S1" s="33" t="s">
+        <v>356</v>
+      </c>
+      <c r="T1" s="33" t="s">
         <v>357</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>358</v>
-      </c>
-      <c r="U1" s="33" t="s">
-        <v>359</v>
       </c>
       <c r="V1" s="33" t="s">
         <v>175</v>
@@ -2707,28 +2729,28 @@
         <v>345</v>
       </c>
       <c r="X1" s="33" t="s">
-        <v>177</v>
+        <v>370</v>
       </c>
       <c r="Y1" s="33" t="s">
-        <v>176</v>
+        <v>371</v>
       </c>
       <c r="Z1" s="34" t="s">
         <v>347</v>
       </c>
       <c r="AA1" s="40" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB1" s="41" t="s">
         <v>360</v>
       </c>
-      <c r="AB1" s="41" t="s">
+      <c r="AC1" s="40" t="s">
         <v>361</v>
       </c>
-      <c r="AC1" s="40" t="s">
+      <c r="AD1" s="40" t="s">
         <v>362</v>
       </c>
-      <c r="AD1" s="40" t="s">
+      <c r="AE1" s="42" t="s">
         <v>363</v>
-      </c>
-      <c r="AE1" s="42" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -2828,22 +2850,22 @@
     </row>
     <row r="3" spans="1:31">
       <c r="A3" s="37" t="s">
+        <v>364</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>365</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>366</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>181</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>350</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G3" s="39">
         <v>20</v>
@@ -2852,10 +2874,10 @@
         <v>0.6</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K3" s="43">
         <v>44.309090909090898</v>
@@ -2928,7 +2950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12184,7 +12206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BK45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20791,7 +20813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21176,7 +21198,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21417,5 +21439,6 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>